<commit_message>
updated audit report added lazy loading in contact.html
</commit_message>
<xml_diff>
--- a/report/audit-SEO deuxieme version.xlsx
+++ b/report/audit-SEO deuxieme version.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="134">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Action recommandée</t>
   </si>
   <si>
-    <t xml:space="preserve">Référence</t>
+    <t xml:space="preserve">Référence (liens hypertexte)</t>
   </si>
   <si>
     <t xml:space="preserve">(SEO ou accessiblité ?)</t>
@@ -73,6 +73,12 @@
     <t xml:space="preserve">&lt;meta robot =”index,follow” &gt; + ajouter un plan du site (sitemap.xml)</t>
   </si>
   <si>
+    <t xml:space="preserve">https://developers.google.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO et Accessibilité</t>
+  </si>
+  <si>
     <t xml:space="preserve">Balise meta title sous-utilisée</t>
   </si>
   <si>
@@ -85,10 +91,19 @@
     <t xml:space="preserve">meta name="title" content="La Chouette Agence - Webdesign à Lyon - Création de sites</t>
   </si>
   <si>
+    <t xml:space="preserve">https://developers.google.com/[..]/good-titles-snippets/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Optimization des mots-clés</t>
   </si>
   <si>
-    <t xml:space="preserve">seo</t>
+    <t xml:space="preserve">Les mots-clés utilisés ne sont pas spécialement pertinents et mal utilisés (Abus de word stuffing notamment).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chercher avec des outils spécialisés tels que google keyword planner des nouveaux mots-clés. Toujours utiliser des mots-clés pertinents , cohérents avec votre site. Ecrire d'abord pour les visiteurs, ensuite pour Google. Essayer de dégager des opportunités: des mots-clés ayant en même temps un fort volume de recherche et une faible compétition. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer les anciens mots-clés et les remplacer par des mots-clés plus à même de faire apparait le site en haut de SERP (Search Engine Results Pages)</t>
   </si>
   <si>
     <t xml:space="preserve">Balise meta description sous-utilisée</t>
@@ -102,6 +117,7 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Description de 370 caractères idéalement. Doit donner envie au visiteur de cliquer pour visiter le site. Contient un maximum de mots-clés </t>
     </r>
@@ -111,6 +127,7 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">cohérents </t>
     </r>
@@ -119,6 +136,7 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">avec le site, sans aller jusqu’au WORD STUFFING tres mal vu; si possible avec une faible competition et fort volume de recherche. La cohérence est la clé</t>
     </r>
@@ -127,12 +145,21 @@
     <t xml:space="preserve">La Chouette Agence UX design, votre entreprise de webdesign sur Lyon. Création de site Internet sur Lyon. Pour un design ergonomique, présentant une forte identité graphique et responsive en toute circonstance, contactez notre studio de création graphique et laissez vous guider par notre équipe de webdesigners adaptés aux normes et tendance du design en 2021</t>
   </si>
   <si>
+    <t xml:space="preserve">developers.google.com SEO starter guide</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abus de la balise meta keywords </t>
   </si>
   <si>
     <t xml:space="preserve">obsolete. Ici combiné à du word stuffing s’apparente a du black hat SEO </t>
   </si>
   <si>
+    <t xml:space="preserve">Suprrimer la balise keyword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developers.google.com/search/docs/advanced/guidelines/irrelevant-keywords</t>
+  </si>
+  <si>
     <t xml:space="preserve">class= keyword  mots clés non optimisé et qui ne s’affichent pas==&gt; word stuffing </t>
   </si>
   <si>
@@ -145,7 +172,10 @@
     <t xml:space="preserve">Supprimer intégralement toutes les itérations de class=”keyword” c’est-à-dire le texte qui ne s’affiche pas</t>
   </si>
   <si>
-    <t xml:space="preserve">broken link</t>
+    <t xml:space="preserve">https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liens morts</t>
   </si>
   <si>
     <t xml:space="preserve">Nous avons sur le site plusieurs liens morts, donnant lieu à des erreurs 404, ce qui est très mauvais en termes de SEO</t>
@@ -161,6 +191,12 @@
   </si>
   <si>
     <t xml:space="preserve">doit être si possible comprehensible et avec moins de 144 caractères</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer les urls et noms des photos. Leur donner un nom pertinent, par exemple contact.html ou agence-de-voyage.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developers.google.com</t>
   </si>
   <si>
     <r>
@@ -169,6 +205,7 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Document doesn't use</t>
     </r>
@@ -177,12 +214,16 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> legible font sizes</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Nos textes doivent avoir une taille de 12px mini pour être lisibles</t>
+    <t xml:space="preserve">Les textes doivent avoir une taille de 12px mini pour être lisibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO et Performance</t>
   </si>
   <si>
     <t xml:space="preserve">empty analytics</t>
@@ -194,7 +235,7 @@
     <t xml:space="preserve">Implementer analytics + search console</t>
   </si>
   <si>
-    <t xml:space="preserve">SEO et Accessibilité</t>
+    <t xml:space="preserve">Analytics , dans la version actuelle du site hébergée sur github pages, fait baisser de 6 points le score de performance du site. J'ai laissé pour l'instant la balise inactive entre des commentaire en attendant un déploiement ultérieur.</t>
   </si>
   <si>
     <t xml:space="preserve">images contenant du texte pertinent tronquées en responsive</t>
@@ -236,9 +277,6 @@
     <t xml:space="preserve">Le contenu est structuré avec des titres de differents niveaux</t>
   </si>
   <si>
-    <t xml:space="preserve">sd</t>
-  </si>
-  <si>
     <t xml:space="preserve">page2 html lien layout</t>
   </si>
   <si>
@@ -254,7 +292,7 @@
     <t xml:space="preserve">li nav vide</t>
   </si>
   <si>
-    <t xml:space="preserve">lien vide (possible reliquat d’une ancienne page?)</t>
+    <t xml:space="preserve">balise  vide (possible reliquat d’une ancienne page?)</t>
   </si>
   <si>
     <t xml:space="preserve">Supprimer </t>
@@ -263,21 +301,15 @@
     <t xml:space="preserve">rediger des contenus performants</t>
   </si>
   <si>
+    <t xml:space="preserve">Il n'y à présentement aucun contenu enrichi. </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Permet l’ajout d’un tas de données utiles et enrichies sur les pages de résultats telles que l’adresse physique, téléphone, reviews yelp ou trustpilot, fiches produits</t>
   </si>
   <si>
     <t xml:space="preserve">Ajouter les informations pertinentes telle que le nom, image, addresse physique et horaires d’ouverture.</t>
   </si>
   <si>
-    <t xml:space="preserve">augmenter l’autorité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trustpilot, yelp , …. réseaux sociaux repondre aux review positive gérez les negatives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEO on page</t>
-  </si>
-  <si>
     <t xml:space="preserve">Titres h1</t>
   </si>
   <si>
@@ -299,7 +331,13 @@
     <t xml:space="preserve">Ne doivent pas être trop lourdes ni downscaled. Utiliser si besoin plusieurs résolutions. Vérifier les balises alt, contenant si possibles le mot-clé dans la mesure du possible.</t>
   </si>
   <si>
-    <t xml:space="preserve">Compresser les images, utiliser des formats modernes (bien plus performants en termes de compression), utiliser plusieurs résolutions si besoin. On peut aussi preload (voir charger les images à la volée) certaines image pour améliorer la performance</t>
+    <t xml:space="preserve">Compresser les images, utiliser des formats modernes (bien plus performants en termes de compression), utiliser plusieurs résolutions si besoin. On peut aussi lazy-load les image, ce qui consiste à charger dynamiquement les images lorsqu'elles s'approchent du viewport. Les images utilisées doivent en outre avoir une taille définie pour éviter un recalcul subséquent du layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nos images sont passées au format webp, compressées et disponibilisées sous différentes résolutions. Elles sont de plus "lazy-loaded" nativement pour les balises img ou grace à du Javascript pour les background en css. Le gain de performance est considérable (cf rapport d'optimisation).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">developer.google.com/search/docs/advanced/javascript/lazy-loading</t>
   </si>
   <si>
     <t xml:space="preserve">Cohérence et longueur de contenu</t>
@@ -314,37 +352,68 @@
     <t xml:space="preserve">Forte concurrence et / ou faible volume de recherche sur les mots-clés ciblés. CF keyword spreadsheet.  Vérifier que l’évolution du trafic va dans le bon sens et est au minimum stable (resultats apparents apres 10 jours)</t>
   </si>
   <si>
+    <t xml:space="preserve">Effectuer une recherche de mots-clés avec leur volume de recherche et concurrence associée. Examinez les positions des mots-clés utilisés et dégager des opportunités (i.e mots-clés possédant un fort volume de recherche et faible compétition)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remplacer les mots-clés utilisés par d'autres plus pertinents et possédant une plus faible compétition.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Créer une machine à contenu</t>
   </si>
   <si>
     <t xml:space="preserve">Plus on a du contenu de qualité plus plus on a de pages indexées par Google et donc de portes d’entrées potentielles . Actualités, expertises, fonctionnement / démonstration de produit newsfeed et/ou de réseaux sociaux, blog</t>
   </si>
   <si>
+    <t xml:space="preserve">Ajouter régulièrement du nouveau contenu</t>
+  </si>
+  <si>
     <t xml:space="preserve">Augmenter l’autorité de votre site (backlink)</t>
   </si>
   <si>
     <t xml:space="preserve">Dépend surtout de la qualité et du nombre de liens qui pointent vers votre site</t>
   </si>
   <si>
-    <t xml:space="preserve">Un lien est de bonne qualité s’il: 1- Provient d’un site connu ou de qualité   2- Se trouve dans un contenu cohérent par rapport à votre domaine métier     3 – Amène un vrai trafic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">autres données importantes </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> taux de visiteurs récurrents, taux de conversion, taux de rebond, configuration matérielle utilisée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">images ont une taille définie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si les image n’ont pas de taille définie au chargement le browser doit recalculer le layout  lorsqu’il charge l’image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reduce unused CSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defer / async script cf screen assets, critical files..</t>
+    <t xml:space="preserve">Un lien est de bonne qualité s’il: 1- Provient d’un site connu ou de qualité   2- Se trouve dans un contenu cohérent par rapport à votre domaine métier     3 – Amène un vrai trafic . </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Etablir si possibles des partenariats. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> Entre outre, trustpilot, yelp et autres réseaux sociaux peuvent amener du trafic de qualité vers votre site. Il faut cependant repondre aux review positive gérez les negatives et "soigner" son image sur les réseaux sociaux ou sites de reviews.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer les classes CSS inutilisées / Minifier les fichier css / Javascript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certaines classes CSS implémentées ne sont pas utilisées et rajoutent du temps de chargement inutile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Èliminer le code inutile grâce à un package npm comme purgecss. On peut aussi minifier le code (éliminer tous les espaces et retours à la ligne inutiles)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réduire les fichiers css et javascript à leur plus simple expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les différents scripts dans la balise head sont chargés séquentiellement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les scripts sont chargés séquentiellement et, étant placés dans la balise head, retardent le chargement de la structure de la page (DOM). Le navigateur doit charger l'intégralité des scripts avant de pouvoir commencer à charger le reste de la page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On utilise async ou defer pour éviter que le chargement de scripts ne bloque le chargement du reste du DOM</t>
   </si>
   <si>
     <t xml:space="preserve">ensure fonts remain visible during webfont load</t>
@@ -373,6 +442,7 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Une gestion cohérente du cache évite d'avoir à tout </t>
     </r>
@@ -381,30 +451,43 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">retélécharger  à chaque fois</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">minify JS</t>
-  </si>
-  <si>
     <t xml:space="preserve">w3c validation</t>
   </si>
   <si>
+    <t xml:space="preserve">Bonnes pratiques</t>
+  </si>
+  <si>
     <t xml:space="preserve">utiliser lib a jour</t>
   </si>
   <si>
     <t xml:space="preserve">Vulnerabilités …</t>
   </si>
   <si>
+    <t xml:space="preserve">utiliser des bibliothèques à jour exemptes de vulnérabilités et / ou erreurs</t>
+  </si>
+  <si>
     <t xml:space="preserve">contrast ratio</t>
   </si>
   <si>
     <t xml:space="preserve">L'arrière plan et l'avant plan de certains élement ont des coouleurs trop semblables, ce qui nuit a la visibilité et donc à l'accessibilité des personnes mal voyantes</t>
   </si>
   <si>
+    <t xml:space="preserve">Utiliser des couleurs suffisament différenciées entre l'arrière plan et l'avant pour permet d'avoir des textes plus lisibles même pour des personne possédant une vision déficiente.</t>
+  </si>
+  <si>
     <t xml:space="preserve">mettre des couleurs suffisament différenciées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.whoisaccessible.com/guidelines/wcag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibilité </t>
   </si>
   <si>
     <t xml:space="preserve">pas de controles aria</t>
@@ -426,11 +509,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -451,38 +535,57 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -541,44 +644,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -586,28 +677,36 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -691,509 +790,606 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1:Z948"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="83.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="98.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="83.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="98.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="164.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="103.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="87.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="1" width="12.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="1" width="13.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" s="7" customFormat="true" ht="48.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+    <row r="5" s="8" customFormat="true" ht="48.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" s="7" customFormat="true" ht="48.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="s">
+      <c r="F5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="s">
+    </row>
+    <row r="6" s="8" customFormat="true" ht="48.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" s="7" customFormat="true" ht="48.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" s="8" customFormat="true" ht="48.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="6"/>
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="58.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>48</v>
+        <v>59</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>52</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>56</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
-        <v>57</v>
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1" t="s">
-        <v>58</v>
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>61</v>
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="58.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>85</v>
+        <v>117</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="45.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C42" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2082,34 +2278,17 @@
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1" display="https://developers.google.com/"/>
+    <hyperlink ref="F6" r:id="rId2" display="https://developers.google.com/[..]/good-titles-snippets/"/>
+    <hyperlink ref="F8" r:id="rId3" location="descriptionmeta" display="developers.google.com SEO starter guide"/>
+    <hyperlink ref="F9" r:id="rId4" display="https://developers.google.com/search/docs/advanced/guidelines/irrelevant-keywords"/>
+    <hyperlink ref="F10" r:id="rId5" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links"/>
+    <hyperlink ref="F12" r:id="rId6" display="https://developers.google.com"/>
+    <hyperlink ref="F24" r:id="rId7" display="developer.google.com/search/docs/advanced/javascript/lazy-loading"/>
+    <hyperlink ref="F36" r:id="rId8" display="https://www.whoisaccessible.com/guidelines/wcag"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>